<commit_message>
[TODO-35]-[Modified]: DefaultProjectManagement Thiết kế xử lý
</commit_message>
<xml_diff>
--- a/ToDoApp-Doc/Document/Diagram/Thiết Kế Phần Mềm/Thiết Kế Xử Lý/DefaultProjectManagement/Thiết-Kế-Xử-Lý.xlsx
+++ b/ToDoApp-Doc/Document/Diagram/Thiết Kế Phần Mềm/Thiết Kế Xử Lý/DefaultProjectManagement/Thiết-Kế-Xử-Lý.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="105">
   <si>
     <t>DANH SÁCH CÁC KIỂU DỮ LIỆU XỬ LÝ</t>
   </si>
@@ -278,11 +278,29 @@
     <t>Loại Dự án mặc định mà người dùng chọn.</t>
   </si>
   <si>
+    <t>createInboxList()</t>
+  </si>
+  <si>
+    <t>Danh sách các Task của Dự án Inbox.</t>
+  </si>
+  <si>
+    <t>Tạo và lưu danh sách các Task của Inbox.</t>
+  </si>
+  <si>
     <t>HashMap</t>
   </si>
   <si>
     <t>Danh sách Task của Dự án mặc định
 đang hiển thị.</t>
+  </si>
+  <si>
+    <t>createTodayList()</t>
+  </si>
+  <si>
+    <t>Danh sách các Task của Dự án Today.</t>
+  </si>
+  <si>
+    <t>Tạo và lưu danh sách các Task của Today.</t>
   </si>
   <si>
     <t>Time</t>
@@ -291,10 +309,37 @@
     <t>Khoảng thời gian cho đến khi kết thúc Task.</t>
   </si>
   <si>
+    <t>createTomorrowList()</t>
+  </si>
+  <si>
+    <t>Danh sách các Task của Dự án Tomorrow.</t>
+  </si>
+  <si>
+    <t>Tạo và lưu danh sách các Task của Tomorrow.</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
     <t>Thời gian tạo và kết thúc của một Task.</t>
+  </si>
+  <si>
+    <t>createWeekList()</t>
+  </si>
+  <si>
+    <t>Danh sách các Task của Dự án Week.</t>
+  </si>
+  <si>
+    <t>Tạo và lưu danh sách các Task của Week.</t>
+  </si>
+  <si>
+    <t>createUpcomingList()</t>
+  </si>
+  <si>
+    <t>Danh sách các Task của Dự án Upcoming.</t>
+  </si>
+  <si>
+    <t>Tạo và lưu danh sách các Task của Upcoming.</t>
   </si>
 </sst>
 </file>
@@ -302,10 +347,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -336,14 +381,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -358,15 +403,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -381,6 +433,45 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -388,34 +479,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -426,10 +494,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -449,22 +518,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -472,15 +525,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -495,7 +540,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -507,37 +696,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -555,127 +720,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -879,11 +924,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -897,17 +948,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -937,21 +988,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -965,151 +1001,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1248,11 +1293,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1584,8 +1627,8 @@
   </sheetPr>
   <dimension ref="A1:AF1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:D1"/>
+    <sheetView tabSelected="1" topLeftCell="U10" workbookViewId="0">
+      <selection activeCell="AE17" sqref="AE17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15.75" customHeight="1"/>
@@ -2252,7 +2295,7 @@
       </c>
       <c r="AF11" s="46"/>
     </row>
-    <row r="12" ht="26.25" customHeight="1" spans="1:32">
+    <row r="12" ht="57" customHeight="1" spans="1:32">
       <c r="A12" s="16">
         <v>6</v>
       </c>
@@ -2290,20 +2333,32 @@
       <c r="W12" s="37"/>
       <c r="X12" s="37"/>
       <c r="Y12" s="5"/>
-      <c r="Z12" s="23"/>
-      <c r="AA12" s="23"/>
-      <c r="AB12" s="48"/>
-      <c r="AC12" s="49"/>
-      <c r="AD12" s="48"/>
-      <c r="AE12" s="49"/>
-      <c r="AF12" s="48"/>
+      <c r="Z12" s="20">
+        <v>10</v>
+      </c>
+      <c r="AA12" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB12" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC12" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="AD12" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE12" s="47" t="s">
+        <v>86</v>
+      </c>
+      <c r="AF12" s="46"/>
     </row>
     <row r="13" ht="50" customHeight="1" spans="1:32">
       <c r="A13" s="11">
         <v>7</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="5"/>
@@ -2324,7 +2379,7 @@
         <v>33</v>
       </c>
       <c r="P13" s="26" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="Q13" s="20"/>
       <c r="R13" s="5"/>
@@ -2335,23 +2390,35 @@
       <c r="W13" s="37"/>
       <c r="X13" s="37"/>
       <c r="Y13" s="5"/>
-      <c r="Z13" s="23"/>
-      <c r="AA13" s="23"/>
-      <c r="AB13" s="48"/>
-      <c r="AC13" s="49"/>
-      <c r="AD13" s="48"/>
-      <c r="AE13" s="49"/>
-      <c r="AF13" s="48"/>
-    </row>
-    <row r="14" ht="32" customHeight="1" spans="1:32">
+      <c r="Z13" s="20">
+        <v>11</v>
+      </c>
+      <c r="AA13" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB13" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC13" s="47" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD13" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE13" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF13" s="46"/>
+    </row>
+    <row r="14" ht="47" customHeight="1" spans="1:32">
       <c r="A14" s="7">
         <v>8</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="5"/>
@@ -2375,23 +2442,35 @@
       <c r="W14" s="37"/>
       <c r="X14" s="37"/>
       <c r="Y14" s="5"/>
-      <c r="Z14" s="23"/>
-      <c r="AA14" s="23"/>
-      <c r="AB14" s="48"/>
-      <c r="AC14" s="49"/>
-      <c r="AD14" s="48"/>
-      <c r="AE14" s="49"/>
-      <c r="AF14" s="48"/>
-    </row>
-    <row r="15" ht="26.25" customHeight="1" spans="1:32">
+      <c r="Z14" s="20">
+        <v>12</v>
+      </c>
+      <c r="AA14" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB14" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC14" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD14" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE14" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="AF14" s="46"/>
+    </row>
+    <row r="15" ht="47" customHeight="1" spans="1:32">
       <c r="A15" s="20">
         <v>9</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="5"/>
@@ -2415,15 +2494,27 @@
       <c r="W15" s="37"/>
       <c r="X15" s="37"/>
       <c r="Y15" s="5"/>
-      <c r="Z15" s="23"/>
-      <c r="AA15" s="23"/>
-      <c r="AB15" s="48"/>
-      <c r="AC15" s="50"/>
-      <c r="AD15" s="51"/>
-      <c r="AE15" s="50"/>
-      <c r="AF15" s="51"/>
-    </row>
-    <row r="16" ht="32" customHeight="1" spans="1:32">
+      <c r="Z15" s="20">
+        <v>13</v>
+      </c>
+      <c r="AA15" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB15" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC15" s="47" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD15" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE15" s="47" t="s">
+        <v>101</v>
+      </c>
+      <c r="AF15" s="48"/>
+    </row>
+    <row r="16" ht="52" customHeight="1" spans="1:32">
       <c r="A16" s="20"/>
       <c r="B16" s="20"/>
       <c r="C16" s="26"/>
@@ -2449,13 +2540,25 @@
       <c r="W16" s="37"/>
       <c r="X16" s="37"/>
       <c r="Y16" s="5"/>
-      <c r="Z16" s="23"/>
-      <c r="AA16" s="23"/>
-      <c r="AB16" s="48"/>
-      <c r="AC16" s="50"/>
-      <c r="AD16" s="51"/>
-      <c r="AE16" s="50"/>
-      <c r="AF16" s="51"/>
+      <c r="Z16" s="20">
+        <v>14</v>
+      </c>
+      <c r="AA16" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB16" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC16" s="47" t="s">
+        <v>103</v>
+      </c>
+      <c r="AD16" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE16" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="AF16" s="48"/>
     </row>
     <row r="17" ht="26.25" customHeight="1" spans="1:32">
       <c r="A17" s="23"/>
@@ -2485,7 +2588,7 @@
       <c r="Y17" s="5"/>
       <c r="Z17" s="23"/>
       <c r="AA17" s="23"/>
-      <c r="AB17" s="48"/>
+      <c r="AB17" s="49"/>
       <c r="AC17" s="50"/>
       <c r="AD17" s="51"/>
       <c r="AE17" s="50"/>

</xml_diff>

<commit_message>
[TODO-35]-[Add]: UserNotificationManagement Thiết kế xử lý
</commit_message>
<xml_diff>
--- a/ToDoApp-Doc/Document/Diagram/Thiết Kế Phần Mềm/Thiết Kế Xử Lý/DefaultProjectManagement/Thiết-Kế-Xử-Lý.xlsx
+++ b/ToDoApp-Doc/Document/Diagram/Thiết Kế Phần Mềm/Thiết Kế Xử Lý/DefaultProjectManagement/Thiết-Kế-Xử-Lý.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="107">
   <si>
     <t>DANH SÁCH CÁC KIỂU DỮ LIỆU XỬ LÝ</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>Lấy giá trị đại diện cho loại Dự án mặc định sẽ hiển thị và tác động.</t>
+  </si>
+  <si>
+    <t>&gt;= 0</t>
   </si>
   <si>
     <t>taskTotal</t>
@@ -350,9 +353,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -398,15 +401,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -434,16 +429,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -481,13 +476,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -505,6 +493,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -512,9 +508,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -528,7 +523,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -549,7 +552,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -561,7 +642,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -573,67 +672,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -651,19 +690,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -675,7 +708,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -687,43 +720,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -917,16 +920,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -966,21 +969,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1013,151 +1001,166 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1631,7 +1634,7 @@
   <dimension ref="A1:AF1004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15.75" customHeight="1"/>
@@ -1861,7 +1864,9 @@
       <c r="H4" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="26"/>
+      <c r="I4" s="26" t="s">
+        <v>32</v>
+      </c>
       <c r="J4" s="16">
         <v>0</v>
       </c>
@@ -1871,13 +1876,13 @@
         <v>2</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O4" s="7" t="s">
         <v>20</v>
       </c>
       <c r="P4" s="24" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Q4" s="7"/>
       <c r="R4" s="5"/>
@@ -1892,19 +1897,19 @@
         <v>2</v>
       </c>
       <c r="AA4" s="46" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AB4" s="46" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AC4" s="47" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AD4" s="46" t="s">
         <v>30</v>
       </c>
       <c r="AE4" s="47" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AF4" s="46"/>
     </row>
@@ -1932,19 +1937,19 @@
         <v>3</v>
       </c>
       <c r="AA5" s="46" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AB5" s="46" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AC5" s="47" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AD5" s="46" t="s">
         <v>30</v>
       </c>
       <c r="AE5" s="47" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AF5" s="46"/>
     </row>
@@ -1953,28 +1958,28 @@
         <v>2</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="5"/>
       <c r="F6" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L6" s="5"/>
       <c r="M6" s="11">
         <v>4</v>
       </c>
       <c r="N6" s="11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="P6" s="22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="Q6" s="11"/>
       <c r="R6" s="5"/>
@@ -1989,19 +1994,19 @@
         <v>4</v>
       </c>
       <c r="AA6" s="46" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AB6" s="46" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AC6" s="47" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AD6" s="46" t="s">
         <v>30</v>
       </c>
       <c r="AE6" s="47" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AF6" s="46"/>
     </row>
@@ -2010,10 +2015,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="5"/>
@@ -2021,14 +2026,14 @@
         <v>1</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I7" s="22"/>
       <c r="J7" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K7" s="11"/>
       <c r="L7" s="5"/>
@@ -2036,13 +2041,13 @@
         <v>5</v>
       </c>
       <c r="N7" s="11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P7" s="22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q7" s="11"/>
       <c r="R7" s="5"/>
@@ -2057,19 +2062,19 @@
         <v>5</v>
       </c>
       <c r="AA7" s="46" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AB7" s="46" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AC7" s="47" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AD7" s="46" t="s">
         <v>30</v>
       </c>
       <c r="AE7" s="47" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AF7" s="46"/>
     </row>
@@ -2078,10 +2083,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="5"/>
@@ -2096,13 +2101,13 @@
         <v>6</v>
       </c>
       <c r="N8" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="O8" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P8" s="22" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="Q8" s="11"/>
       <c r="R8" s="5"/>
@@ -2117,19 +2122,19 @@
         <v>6</v>
       </c>
       <c r="AA8" s="46" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AB8" s="46" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AC8" s="47" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AD8" s="46" t="s">
         <v>30</v>
       </c>
       <c r="AE8" s="47" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AF8" s="46"/>
     </row>
@@ -2138,10 +2143,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="5"/>
@@ -2156,13 +2161,13 @@
         <v>7</v>
       </c>
       <c r="N9" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O9" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P9" s="22" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Q9" s="11"/>
       <c r="R9" s="5"/>
@@ -2177,19 +2182,19 @@
         <v>7</v>
       </c>
       <c r="AA9" s="46" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AB9" s="46" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AC9" s="47" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AD9" s="46" t="s">
         <v>30</v>
       </c>
       <c r="AE9" s="47" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AF9" s="46"/>
     </row>
@@ -2210,13 +2215,13 @@
         <v>8</v>
       </c>
       <c r="N10" s="11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O10" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P10" s="22" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Q10" s="11"/>
       <c r="R10" s="5"/>
@@ -2231,19 +2236,19 @@
         <v>8</v>
       </c>
       <c r="AA10" s="46" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AB10" s="46" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AC10" s="47" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AD10" s="46" t="s">
         <v>30</v>
       </c>
       <c r="AE10" s="47" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AF10" s="46"/>
     </row>
@@ -2264,13 +2269,13 @@
         <v>9</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="O11" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P11" s="24" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="Q11" s="7"/>
       <c r="R11" s="5"/>
@@ -2285,19 +2290,19 @@
         <v>9</v>
       </c>
       <c r="AA11" s="46" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AB11" s="46" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AC11" s="47" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AD11" s="46" t="s">
         <v>30</v>
       </c>
       <c r="AE11" s="47" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AF11" s="46"/>
     </row>
@@ -2306,7 +2311,7 @@
         <v>6</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C12" s="22"/>
       <c r="D12" s="17"/>
@@ -2328,7 +2333,7 @@
         <v>20</v>
       </c>
       <c r="P12" s="31" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="Q12" s="38"/>
       <c r="R12" s="5"/>
@@ -2343,19 +2348,19 @@
         <v>10</v>
       </c>
       <c r="AA12" s="16" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AB12" s="46" t="s">
         <v>28</v>
       </c>
       <c r="AC12" s="47" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AD12" s="46" t="s">
         <v>30</v>
       </c>
       <c r="AE12" s="47" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AF12" s="46"/>
     </row>
@@ -2364,7 +2369,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="5"/>
@@ -2379,13 +2384,13 @@
         <v>11</v>
       </c>
       <c r="N13" s="16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="O13" s="16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P13" s="26" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Q13" s="16"/>
       <c r="R13" s="5"/>
@@ -2400,19 +2405,19 @@
         <v>11</v>
       </c>
       <c r="AA13" s="16" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AB13" s="46" t="s">
         <v>28</v>
       </c>
       <c r="AC13" s="47" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AD13" s="46" t="s">
         <v>30</v>
       </c>
       <c r="AE13" s="47" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AF13" s="46"/>
     </row>
@@ -2421,10 +2426,10 @@
         <v>8</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="5"/>
@@ -2452,19 +2457,19 @@
         <v>12</v>
       </c>
       <c r="AA14" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AB14" s="46" t="s">
         <v>28</v>
       </c>
       <c r="AC14" s="47" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AD14" s="46" t="s">
         <v>30</v>
       </c>
       <c r="AE14" s="47" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AF14" s="46"/>
     </row>
@@ -2473,10 +2478,10 @@
         <v>9</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="5"/>
@@ -2504,19 +2509,19 @@
         <v>13</v>
       </c>
       <c r="AA15" s="16" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AB15" s="46" t="s">
         <v>28</v>
       </c>
       <c r="AC15" s="47" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AD15" s="46" t="s">
         <v>30</v>
       </c>
       <c r="AE15" s="47" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AF15" s="48"/>
     </row>
@@ -2550,19 +2555,19 @@
         <v>14</v>
       </c>
       <c r="AA16" s="16" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AB16" s="46" t="s">
         <v>28</v>
       </c>
       <c r="AC16" s="47" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AD16" s="46" t="s">
         <v>30</v>
       </c>
       <c r="AE16" s="47" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AF16" s="48"/>
     </row>

</xml_diff>